<commit_message>
Added new column to participants excel
</commit_message>
<xml_diff>
--- a/orden_pruebas_participantes.xlsx
+++ b/orden_pruebas_participantes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc2\Proyecto_Alphamini\python-alphamini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A65F2EB-55AE-4D76-80BD-F57406454744}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B29496-8BF6-48C1-8E80-F7DEF61907DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="8">
   <si>
     <t>Participante</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Realidad Virtual</t>
+  </si>
+  <si>
+    <t>Fecha</t>
   </si>
 </sst>
 </file>
@@ -69,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -92,17 +95,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,18 +425,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -430,8 +450,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -445,7 +468,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -459,7 +482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -473,7 +496,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -487,7 +510,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -501,7 +524,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -515,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -529,7 +552,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -543,7 +566,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -557,7 +580,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -571,7 +594,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -585,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -599,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -613,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -627,7 +650,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>

</xml_diff>